<commit_message>
added images, fixed css...
to fit in new FAQ icon on homepage
</commit_message>
<xml_diff>
--- a/db-import-dm-edits-for-upload-august-2015-test1.xlsx
+++ b/db-import-dm-edits-for-upload-august-2015-test1.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24120" windowHeight="11985"/>
+    <workbookView xWindow="10335" yWindow="105" windowWidth="13665" windowHeight="10605"/>
   </bookViews>
   <sheets>
     <sheet name="databases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
   <si>
     <t>VENDOR NAME</t>
   </si>
@@ -173,13 +173,85 @@
   </si>
   <si>
     <t>http://0-library.artstor.org.helin.uri.edu/library/#1</t>
+  </si>
+  <si>
+    <t>Boston Globe (ProQuest)</t>
+  </si>
+  <si>
+    <t>A New England regional newspaper. Selective, full-text daily coverage from 1980 - Present of news articles and opinion editorials written or edited by the Globe's staff. This is text-based only; images are not available.</t>
+  </si>
+  <si>
+    <t>Business Education in Video (Alex. St. Press)</t>
+  </si>
+  <si>
+    <t>Streaming video clips ranging from 2-10 min. feature executive interviews, corporate training, and case studies for both small to large business firms globally. Coverage includes Cross-Cultural Communication, Ethics, Negotiations, Operations &amp; Logistics, Technology, and more. You can also use the Advanced Search link to focus on a specialized area of interest such as Accounting, Consumer Behavior, Corporate Communication, Corporate Governance, Economics, Entrepreneurship, Finance, Human Resource Management, International Business, Marketing Strategy, Strategic Management, and Supply Chain Management.</t>
+  </si>
+  <si>
+    <t>Business Insights: Global (Gale)</t>
+  </si>
+  <si>
+    <t>Comprehensive business content including case studies, company profiles &amp; industry research reports, country economic reports, market research reports, SWOT analyses, and video interviews with business executives. (formerly, Business &amp; Company Resource Center)</t>
+  </si>
+  <si>
+    <t>Business Plans Handbooks (Gale)  </t>
+  </si>
+  <si>
+    <t>Are you planning to start a small business? This is a collection of actual business plans submitted by entrepreneurs in North America (company names and addresses have been changed). Each volume also includes a business plan template, a listing of organizations, agencies &amp; consultants, and glossary. NOTE: You can keyword search across ALL of JWU's purchased volumes to date to find a plan for a specific type of business, for example, by entering the word "restaurant." Plans are from businesses in the manufacturing, retail and service industries and include both traditional businesses and new types of start-ups such as a Cloud Computing Business or an iPhone App Developer. Click on the "i" icon for more examples of the types of businesses represented.</t>
+  </si>
+  <si>
+    <t>Business Source Complete (EBSCO)</t>
+  </si>
+  <si>
+    <t>Company profiles, SWOT analyses (Strengths, Weaknesses, Opportunities, Threats) where available, industry profiles, stocks &amp; investment info., management-related articles, Harvard Business Review case studies and streaming videos from the Harvard Business School Faculty Seminar Series.</t>
+  </si>
+  <si>
+    <t>http://0-www.bergfashionlibrary.com.helin.uri.edu/</t>
+  </si>
+  <si>
+    <t>http://0-infotrac.galegroup.com.helin.uri.edu/itweb/prov43712?db=BIC1</t>
+  </si>
+  <si>
+    <t>http://0-search.proquest.com.helin.uri.edu/biologicalscience?accountid=1363</t>
+  </si>
+  <si>
+    <t>Berg Fashion Library (Oxford Univ. Press)</t>
+  </si>
+  <si>
+    <t>International in scope, thousands of images plus key fashion reference sources including Encyclopedia of World Dress and Fashion, A-Z of Fashion, Dictionary of Fashion History, &amp; nearly 60 fashion e-books (from the "Subscribers" column), and selective journal articles. "Explore by Time &amp; Place" and also browse by Dress, People &amp; Organizations, Period, Textiles &amp; Materials, The Fashion Industry, and Themes.</t>
+  </si>
+  <si>
+    <t>http://0-search.proquest.com.helin.uri.edu/bostonglobe/advanced?accountid=1363</t>
+  </si>
+  <si>
+    <t>Biography In Context (Gale)</t>
+  </si>
+  <si>
+    <t>Biographies of people worldwide in many fields throughout history: artists, authors, business leaders, chefs, government leaders &amp; politicians, historical figures, popular entertainers, scientists, sports figures, and people currently in the news.</t>
+  </si>
+  <si>
+    <t>Biological Science Collection (ProQuest)</t>
+  </si>
+  <si>
+    <t>Selected full text from over 6,000 journal titles, conference proceedings, technical reports, books and patents. Subject areas include research in Animal Behavior, Bacteriology, Biotechnology, Ecology, Human Genome, Immunology, Micro &amp; Molecular Biology, Safety Science, Toxicology, Veterinary Science &amp; Zoology.</t>
+  </si>
+  <si>
+    <t>http://0-search.alexanderstreet.com.helin.uri.edu/busv</t>
+  </si>
+  <si>
+    <t>http://0-infotrac.galegroup.com.helin.uri.edu/itweb/prov43712?db=BIG</t>
+  </si>
+  <si>
+    <t>http://0-go.galegroup.com.helin.uri.edu/ps/i.do?id=0PHU&amp;v=2.1&amp;u=prov43712&amp;it=aboutSeries&amp;p=GVRL&amp;sw=w</t>
+  </si>
+  <si>
+    <t>http://0-search.ebscohost.com.helin.uri.edu/login.aspx?authtype=ip,uid&amp;profile=bsi&amp;defaultdb=bth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +280,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -230,7 +309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -241,6 +320,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -546,15 +631,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="104" customWidth="1"/>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" customWidth="1"/>
     <col min="4" max="4" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.28515625" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
@@ -614,7 +699,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="72" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
@@ -682,7 +767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="96" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>32</v>
       </c>
@@ -716,7 +801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="96" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
@@ -733,7 +818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="96" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="276" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>21</v>
       </c>
@@ -784,54 +869,226 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" ht="168" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C16" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="24" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="24" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C18" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="171" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="72" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="96" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="84" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="216" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="84" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
         <v>0</v>
       </c>
     </row>
@@ -868,13 +1125,19 @@
     <hyperlink ref="B10" r:id="rId7" display="http://0-accessmedicine.mhmedical.com.helin.uri.edu/"/>
     <hyperlink ref="B11" r:id="rId8" display="http://0-www.humanitiesebook.org.helin.uri.edu/"/>
     <hyperlink ref="B12" r:id="rId9" display="http://0-dl.acm.org.helin.uri.edu/"/>
-    <hyperlink ref="B13" r:id="rId10" display="http://0-www.redbooks.com.helin.uri.edu/dotCMS/validateLogin?dispatch=siteLogin"/>
-    <hyperlink ref="B14" r:id="rId11" display="http://0-search.ebscohost.com.helin.uri.edu/login.aspx?authtype=ip,uid&amp;profile=ehost&amp;defaultdb=31h"/>
-    <hyperlink ref="B15" r:id="rId12" location="1" display="http://0-library.artstor.org.helin.uri.edu/library/ - 1"/>
+    <hyperlink ref="B16" r:id="rId10" display="http://0-www.redbooks.com.helin.uri.edu/dotCMS/validateLogin?dispatch=siteLogin"/>
+    <hyperlink ref="B17" r:id="rId11" display="http://0-search.ebscohost.com.helin.uri.edu/login.aspx?authtype=ip,uid&amp;profile=ehost&amp;defaultdb=31h"/>
+    <hyperlink ref="B18" r:id="rId12" location="1" display="http://0-library.artstor.org.helin.uri.edu/library/ - 1"/>
     <hyperlink ref="B7" r:id="rId13" display="http://0-www.nutritioncaremanual.org.helin.uri.edu/sso.cfm?c=johnsonw2"/>
+    <hyperlink ref="B23" r:id="rId14" display="http://0-infotrac.galegroup.com.helin.uri.edu/itweb/prov43712?db=BIC1"/>
+    <hyperlink ref="B24" r:id="rId15" display="http://0-search.proquest.com.helin.uri.edu/biologicalscience?accountid=1363"/>
+    <hyperlink ref="B25" r:id="rId16" display="http://0-search.proquest.com.helin.uri.edu/bostonglobe/advanced?accountid=1363"/>
+    <hyperlink ref="B26" r:id="rId17" display="http://0-search.alexanderstreet.com.helin.uri.edu/busv"/>
+    <hyperlink ref="B27" r:id="rId18" display="http://0-infotrac.galegroup.com.helin.uri.edu/itweb/prov43712?db=BIG"/>
+    <hyperlink ref="B28" r:id="rId19" display="http://0-go.galegroup.com.helin.uri.edu/ps/i.do?id=0PHU&amp;v=2.1&amp;u=prov43712&amp;it=aboutSeries&amp;p=GVRL&amp;sw=w"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
databases xml imports, also webscraper attempt
</commit_message>
<xml_diff>
--- a/db-import-dm-edits-for-upload-august-2015-test1.xlsx
+++ b/db-import-dm-edits-for-upload-august-2015-test1.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10335" yWindow="105" windowWidth="13665" windowHeight="10605"/>
+    <workbookView xWindow="10335" yWindow="105" windowWidth="13665" windowHeight="10605" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="databases" sheetId="1" r:id="rId1"/>
+    <sheet name="a" sheetId="1" r:id="rId1"/>
+    <sheet name="b" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
   <si>
     <t>VENDOR NAME</t>
   </si>
@@ -245,13 +246,19 @@
   </si>
   <si>
     <t>http://0-search.ebscohost.com.helin.uri.edu/login.aspx?authtype=ip,uid&amp;profile=bsi&amp;defaultdb=bth</t>
+  </si>
+  <si>
+    <t>A brief sampling of the businesses represented include Accounting Service, Banquet Facility, Bed &amp; Breakfast, Biscotti Bakery, Cloud Computing Business, Counseling Practice, Day Spa, Digital Presentations, E-Commerce Website Producer, Early Childhood Program, Event Planning Company, Financial Services Company, Fitness Center, Food &amp; Beverage Vending Company, Gourmet Foods Company, Grant Writer, Horse Riding School, Import Boutique, Information Technology Personnel Agency, iPhone App Developer, Internet Loyalty Program, Internet Travel Agency, Marketing Communications Firm, Men's Clothing Retailer, Microbrewery, Music Festival Promotion, Nightclub, Novelty Shop, Organic Food Store, Outdoor Adventure Travel Company, Party Supply Store, Resale Clothing Store, Restaurant Franchise, Ski Resort, Specialty Food Manufacturer, Sports Bar and Grille, Sports Tournament Organizer, Stable, Steak House, Student Services Consulting Firm, Vegetarian Fast Food Restaurant, Venture Capital &amp; Financing Companies, Video Production &amp; Distribution Company, Virtual Shopping, and Wine Merchant &amp; Storage Facilty.</t>
+  </si>
+  <si>
+    <t>Close</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,6 +294,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF222222"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -309,7 +322,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -325,6 +338,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -631,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H381"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
@@ -852,7 +871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
@@ -898,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="24" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>25</v>
       </c>
@@ -956,140 +975,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="171" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" ht="72" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" ht="96" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" t="s">
-        <v>66</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="180" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" ht="84" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" t="s">
-        <v>72</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="216" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" ht="84" x14ac:dyDescent="0.25">
-      <c r="B29" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" t="s">
-        <v>74</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F30" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="35" ht="86.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1116,32 +1004,249 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="http://0-legacy.abc-clio.com.helin.uri.edu/"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://0-ncpt.webauthor.com.helin.uri.edu/auth.cfm?actionxm=SSO&amp;sso_account_key=0D182635-4531-423B-957D-5937E709CFB3&amp;sso_account_id=95"/>
-    <hyperlink ref="B5" r:id="rId3" display="http://0-www.andevidencelibrary.com.helin.uri.edu/sso.cfm?key=2e4bfdb8-35c8-423b-868a-89c33fbdd285&amp;u=JWU-JWUUSER"/>
-    <hyperlink ref="B6" r:id="rId4" display="http://0-www.nutritioncaremanual.org.helin.uri.edu/sso.cfm?c=johnsonw"/>
-    <hyperlink ref="B8" r:id="rId5" display="http://0-www.nutritioncaremanual.org.helin.uri.edu/sso.cfm?c=johnsonw3"/>
-    <hyperlink ref="B9" r:id="rId6" display="http://0-search.ebscohost.com.helin.uri.edu/login.aspx?authtype=ip,uid&amp;profile=ehost&amp;defaultdb=a9h"/>
-    <hyperlink ref="B10" r:id="rId7" display="http://0-accessmedicine.mhmedical.com.helin.uri.edu/"/>
-    <hyperlink ref="B11" r:id="rId8" display="http://0-www.humanitiesebook.org.helin.uri.edu/"/>
-    <hyperlink ref="B12" r:id="rId9" display="http://0-dl.acm.org.helin.uri.edu/"/>
-    <hyperlink ref="B16" r:id="rId10" display="http://0-www.redbooks.com.helin.uri.edu/dotCMS/validateLogin?dispatch=siteLogin"/>
-    <hyperlink ref="B17" r:id="rId11" display="http://0-search.ebscohost.com.helin.uri.edu/login.aspx?authtype=ip,uid&amp;profile=ehost&amp;defaultdb=31h"/>
-    <hyperlink ref="B18" r:id="rId12" location="1" display="http://0-library.artstor.org.helin.uri.edu/library/ - 1"/>
-    <hyperlink ref="B7" r:id="rId13" display="http://0-www.nutritioncaremanual.org.helin.uri.edu/sso.cfm?c=johnsonw2"/>
-    <hyperlink ref="B23" r:id="rId14" display="http://0-infotrac.galegroup.com.helin.uri.edu/itweb/prov43712?db=BIC1"/>
-    <hyperlink ref="B24" r:id="rId15" display="http://0-search.proquest.com.helin.uri.edu/biologicalscience?accountid=1363"/>
-    <hyperlink ref="B25" r:id="rId16" display="http://0-search.proquest.com.helin.uri.edu/bostonglobe/advanced?accountid=1363"/>
-    <hyperlink ref="B26" r:id="rId17" display="http://0-search.alexanderstreet.com.helin.uri.edu/busv"/>
-    <hyperlink ref="B27" r:id="rId18" display="http://0-infotrac.galegroup.com.helin.uri.edu/itweb/prov43712?db=BIG"/>
-    <hyperlink ref="B28" r:id="rId19" display="http://0-go.galegroup.com.helin.uri.edu/ps/i.do?id=0PHU&amp;v=2.1&amp;u=prov43712&amp;it=aboutSeries&amp;p=GVRL&amp;sw=w"/>
+    <hyperlink ref="B9" r:id="rId1" display="http://0-search.ebscohost.com.helin.uri.edu/login.aspx?authtype=ip,uid&amp;profile=ehost&amp;defaultdb=a9h"/>
+    <hyperlink ref="B10" r:id="rId2" display="http://0-accessmedicine.mhmedical.com.helin.uri.edu/"/>
+    <hyperlink ref="B11" r:id="rId3" display="http://0-www.humanitiesebook.org.helin.uri.edu/"/>
+    <hyperlink ref="B12" r:id="rId4" display="http://0-dl.acm.org.helin.uri.edu/"/>
+    <hyperlink ref="B16" r:id="rId5" display="http://0-www.redbooks.com.helin.uri.edu/dotCMS/validateLogin?dispatch=siteLogin"/>
+    <hyperlink ref="B17" r:id="rId6" display="http://0-search.ebscohost.com.helin.uri.edu/login.aspx?authtype=ip,uid&amp;profile=ehost&amp;defaultdb=31h"/>
+    <hyperlink ref="B18" r:id="rId7" location="1" display="http://0-library.artstor.org.helin.uri.edu/library/ - 1"/>
+    <hyperlink ref="F30" r:id="rId8" display="http://jwu-ri.v1.libguides.com/friendly.php?s=databasesbyname"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="360" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="324" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="372" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1">
+      <formula1>5000</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
+      <formula1>500</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:D1">
+      <formula1>1000</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>255</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B9" r:id="rId1" display="http://0-go.galegroup.com.helin.uri.edu/ps/i.do?id=0PHU&amp;v=2.1&amp;u=prov43712&amp;it=aboutSeries&amp;p=GVRL&amp;sw=w"/>
+    <hyperlink ref="B8" r:id="rId2" display="http://0-infotrac.galegroup.com.helin.uri.edu/itweb/prov43712?db=BIG"/>
+    <hyperlink ref="B7" r:id="rId3" display="http://0-search.alexanderstreet.com.helin.uri.edu/busv"/>
+    <hyperlink ref="B6" r:id="rId4" display="http://0-search.proquest.com.helin.uri.edu/bostonglobe/advanced?accountid=1363"/>
+    <hyperlink ref="B5" r:id="rId5" display="http://0-search.proquest.com.helin.uri.edu/biologicalscience?accountid=1363"/>
+    <hyperlink ref="B4" r:id="rId6" display="http://0-infotrac.galegroup.com.helin.uri.edu/itweb/prov43712?db=BIC1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>